<commit_message>
multiple menu headers (themes)
</commit_message>
<xml_diff>
--- a/sli_measures.xlsx
+++ b/sli_measures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa0eda03202f8011/BI/Repo/asc-localities-insight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_CF605FDF8F79A8D366075C52F37BD2724A4BF33F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD9CC414-47E1-4892-A70C-04C4932C3347}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_CF605FDF8F79A8D366075C52F37BD2724A4BF33F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6386002F-9BCF-435D-8807-A1E74F4DA733}"/>
   <bookViews>
-    <workbookView xWindow="-57120" yWindow="-120" windowWidth="28440" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="444" yWindow="-108" windowWidth="22704" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="265">
   <si>
     <t>theme</t>
   </si>
@@ -1208,8 +1208,8 @@
   <dimension ref="A1:C260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B272" sqref="B272"/>
+      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J224" sqref="J224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1230,7 +1230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>3</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>3</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>3</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>3</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>3</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>3</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>3</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>3</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>3</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>3</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>3</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>3</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>3</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>3</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>3</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>3</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>3</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>3</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>3</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>3</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>3</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>3</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>3</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>3</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>3</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>3</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>3</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>3</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>3</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>3</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>3</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>3</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>3</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>3</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>3</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>3</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>3</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>3</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>3</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>3</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>3</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>3</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>3</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>3</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>3</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>3</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>3</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>3</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>3</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>3</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>3</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>3</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>3</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>3</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>3</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>3</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>3</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>3</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>3</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>3</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>3</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>3</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>3</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>3</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>184</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>184</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>184</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>184</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>184</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>184</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>184</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>184</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>184</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>184</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>184</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>184</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>184</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>184</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>184</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>184</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>184</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>184</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>184</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>184</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>184</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>184</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>184</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>184</v>
       </c>
@@ -2876,7 +2876,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>184</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>184</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>184</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>184</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>184</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>184</v>
       </c>
@@ -2924,15 +2924,18 @@
         <v>215</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>184</v>
       </c>
       <c r="B213" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C213" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>184</v>
       </c>
@@ -2940,7 +2943,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>184</v>
       </c>
@@ -2948,7 +2951,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>184</v>
       </c>
@@ -2956,7 +2959,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>184</v>
       </c>
@@ -2964,7 +2967,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>184</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>184</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>184</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>184</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>184</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>184</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>184</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>184</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>184</v>
       </c>
@@ -3036,7 +3039,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>184</v>
       </c>
@@ -3044,7 +3047,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>184</v>
       </c>
@@ -3052,7 +3055,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>184</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>184</v>
       </c>
@@ -3068,7 +3071,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>184</v>
       </c>
@@ -3076,7 +3079,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>184</v>
       </c>
@@ -3084,7 +3087,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>184</v>
       </c>
@@ -3092,7 +3095,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>184</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>184</v>
       </c>
@@ -3108,7 +3111,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>184</v>
       </c>
@@ -3116,7 +3119,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>184</v>
       </c>
@@ -3124,7 +3127,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>184</v>
       </c>
@@ -3132,7 +3135,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>184</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>184</v>
       </c>
@@ -3148,7 +3151,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>184</v>
       </c>
@@ -3156,7 +3159,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>184</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>184</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>184</v>
       </c>
@@ -3180,7 +3183,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>184</v>
       </c>
@@ -3188,7 +3191,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>184</v>
       </c>
@@ -3196,7 +3199,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>184</v>
       </c>
@@ -3204,7 +3207,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>184</v>
       </c>
@@ -3212,7 +3215,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>184</v>
       </c>
@@ -3220,7 +3223,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>184</v>
       </c>
@@ -3228,7 +3231,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>184</v>
       </c>
@@ -3236,7 +3239,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>184</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>184</v>
       </c>
@@ -3252,7 +3255,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>184</v>
       </c>
@@ -3260,7 +3263,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>184</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>184</v>
       </c>
@@ -3276,7 +3279,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>184</v>
       </c>
@@ -3284,7 +3287,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>184</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>184</v>
       </c>
@@ -3300,7 +3303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>184</v>
       </c>
@@ -3312,7 +3315,7 @@
   <autoFilter ref="A1:C260" xr:uid="{EF5AA1A9-BF36-4E01-8C1C-DF384EC058C4}">
     <filterColumn colId="0">
       <filters>
-        <filter val="population"/>
+        <filter val="deprivation"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
iterate over separate data exports of SLI themes
</commit_message>
<xml_diff>
--- a/sli_measures.xlsx
+++ b/sli_measures.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa0eda03202f8011/BI/Repo/asc-localities-insight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_CF605FDF8F79A8D366075C52F37BD2724A4BF33F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6386002F-9BCF-435D-8807-A1E74F4DA733}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_AE351DC08F79A8D366075C52F37BD2727A472C54" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0B922AA-8196-47A6-972A-506837EED5F6}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="-108" windowWidth="22704" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57120" yWindow="-120" windowWidth="28440" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$386</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="392">
   <si>
     <t>theme</t>
   </si>
@@ -34,6 +34,627 @@
     <t>include</t>
   </si>
   <si>
+    <t>deprivation</t>
+  </si>
+  <si>
+    <t>Children 0-19 in absolute low-income couple families (as % of all in absolute low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in absolute low-income in-work families (as % of all in absolute low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in absolute low-income lone parent families (as % of all in absolute low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in absolute low-income out of work families (as % of all in absolute low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in relative low-income couple families (as % of all in relative low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in relative low-income in-work families (as % of all in relative low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in relative low-income lone parent families (as % of all in relative low income families)</t>
+  </si>
+  <si>
+    <t>Children 0-19 in relative low-income out of work families (as % of all in relative low income families)</t>
+  </si>
+  <si>
+    <t>Children aged 0-15 in absolute low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 0-15 in poverty</t>
+  </si>
+  <si>
+    <t>Children aged 0-15 in relative low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 0-19 in absolute low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 0-19 in poverty</t>
+  </si>
+  <si>
+    <t>Children aged 0-19 in relative low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 0-4 in absolute low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 0-4 in poverty</t>
+  </si>
+  <si>
+    <t>Children aged 0-4 in relative low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 11-15 in absolute low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 11-15 in poverty</t>
+  </si>
+  <si>
+    <t>Children aged 11-15 in relative low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 16-19 in absolute low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 16-19 in poverty</t>
+  </si>
+  <si>
+    <t>Children aged 16-19 in relative low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 5-10 in absolute low-income families</t>
+  </si>
+  <si>
+    <t>Children aged 5-10 in poverty</t>
+  </si>
+  <si>
+    <t>Children aged 5-10 in relative low-income families</t>
+  </si>
+  <si>
+    <t>Food Vulnerability Index Score</t>
+  </si>
+  <si>
+    <t>Hardship Fund Vulnerability Index Score</t>
+  </si>
+  <si>
+    <t>Households in Fuel Poverty</t>
+  </si>
+  <si>
+    <t>Households in poverty</t>
+  </si>
+  <si>
+    <t>Index of Multiple Deprivation (IMD) 2019 Rank</t>
+  </si>
+  <si>
+    <t>Index of Multiple Deprivation 2019 (IMD) Score</t>
+  </si>
+  <si>
+    <t>IoD 2019 Acute morbidity indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Adult Skills Sub-domain Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Adult skills and English language proficiency indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Air quality indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Barriers to Housing and Services Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Benzene (component of air quality indicator)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Children and Young People Sub-domain Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Comparative illness and disability ratio indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Crime Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Education, Skills and Training Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Employment Score (rate)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Entry to higher education indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Geographical Barriers Sub-domain Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Health Deprivation and Disability Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Homelessness indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Household overcrowding indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Houses without central heating indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Housing affordability indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Housing in poor condition indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Income Deprivation Affecting Children Index (IDACI) Score (rate)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Income Deprivation Affecting Older People (IDAOPI) Score (rate)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Income Score (rate)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Indoors Sub-domain Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Living Environment Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Mood and anxiety disorders indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Nitrogen dioxide (component of air quality indicator)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Outdoors Sub-domain Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Owner-occupation affordability (component of housing affordability indicator)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Particulates (component of air quality indicator)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Private rental affordability (component of housing affordability indicator)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Road distance to a GP surgery indicator (km)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Road distance to a post office indicator (km)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Road distance to a primary school indicator (km)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Road distance to general store or supermarket indicator (km)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Road traffic accidents indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Staying on in education post 16 indicator</t>
+  </si>
+  <si>
+    <t>IoD 2019 Sulphur dioxide (component of air quality indicator)</t>
+  </si>
+  <si>
+    <t>IoD 2019 Wider Barriers Sub-domain Rank</t>
+  </si>
+  <si>
+    <t>IoD 2019 Years of potential life lost indicator</t>
+  </si>
+  <si>
+    <t>Mortgage debt per household</t>
+  </si>
+  <si>
+    <t>Net annual household income estimate</t>
+  </si>
+  <si>
+    <t>Net annual household income estimate after housing costs</t>
+  </si>
+  <si>
+    <t>Net annual household income estimate before housing costs</t>
+  </si>
+  <si>
+    <t>Percentage of children in poverty (after housing costs)</t>
+  </si>
+  <si>
+    <t>Personal debt (unsecured loans) per person aged 18+</t>
+  </si>
+  <si>
+    <t>Social benefits as a percentage of total household income</t>
+  </si>
+  <si>
+    <t>Total annual household income estimate</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>Adults who are physically active (modelled MSOA estimates)  (2016/17)</t>
+  </si>
+  <si>
+    <t>Adults who are physically active (modelled MSOA estimates) (2017/18)</t>
+  </si>
+  <si>
+    <t>Adults who are physically active (modelled MSOA estimates) (2018/19)</t>
+  </si>
+  <si>
+    <t>Adults who are physically inactive (modelled MSOA estimates)  (2016/17)</t>
+  </si>
+  <si>
+    <t>Adults who are physically inactive (modelled MSOA estimates) (2017/18)</t>
+  </si>
+  <si>
+    <t>Adults who are physically inactive (modelled MSOA estimates) (2018/19)</t>
+  </si>
+  <si>
+    <t>Asthma prevalence</t>
+  </si>
+  <si>
+    <t>Atrial Fibrillation prevalence</t>
+  </si>
+  <si>
+    <t>Average anxiety score (where 0 is 'not at all anxious' and 10 is 'completely anxious')</t>
+  </si>
+  <si>
+    <t>Average happiness score (where 0 is 'not at all happy' and 10 is 'completely happy')</t>
+  </si>
+  <si>
+    <t>Average life satisfaction score (where 0 is 'not at all satisfied' and 10 is 'completely satisfied')</t>
+  </si>
+  <si>
+    <t>Average worthwhile score (where 0 is 'not at all worthwhile' and 10 is 'completely worthwhile')</t>
+  </si>
+  <si>
+    <t>Bad health</t>
+  </si>
+  <si>
+    <t>Binge drinking</t>
+  </si>
+  <si>
+    <t>COPD prevalence</t>
+  </si>
+  <si>
+    <t>COVID-19 vulnerability index (MSOA Level)</t>
+  </si>
+  <si>
+    <t>Cancer incidence</t>
+  </si>
+  <si>
+    <t>Cancer prevalence (diagnosis since 2003)</t>
+  </si>
+  <si>
+    <t>Cardiovascular Disease prevalence</t>
+  </si>
+  <si>
+    <t>Chronic Kidney Disease prevalence</t>
+  </si>
+  <si>
+    <t>Coronary Heart Disease prevalence</t>
+  </si>
+  <si>
+    <t>Day-to-day activities limited a little</t>
+  </si>
+  <si>
+    <t>Day-to-day activities limited a little: Age 16 to 64</t>
+  </si>
+  <si>
+    <t>Day-to-day activities limited a lot</t>
+  </si>
+  <si>
+    <t>Day-to-day activities limited a lot: Age 16 to 64</t>
+  </si>
+  <si>
+    <t>Deaths (all causes)</t>
+  </si>
+  <si>
+    <t>Deaths all ages, circulatory disease</t>
+  </si>
+  <si>
+    <t>Deaths all ages, coronary heart disease (CHD)</t>
+  </si>
+  <si>
+    <t>Deaths all ages, respiratory disease</t>
+  </si>
+  <si>
+    <t>Deaths all ages, stroke</t>
+  </si>
+  <si>
+    <t>Deaths from cancer</t>
+  </si>
+  <si>
+    <t>Deaths under 65, all causes</t>
+  </si>
+  <si>
+    <t>Deaths under 75, all cancers</t>
+  </si>
+  <si>
+    <t>Deaths under 75, all causes</t>
+  </si>
+  <si>
+    <t>Deaths under 75, circulatory disease</t>
+  </si>
+  <si>
+    <t>Deaths under 75, coronary heart disease (CHD)</t>
+  </si>
+  <si>
+    <t>Dementia prevalence</t>
+  </si>
+  <si>
+    <t>Depression prevalence</t>
+  </si>
+  <si>
+    <t>Diabetes prevalence</t>
+  </si>
+  <si>
+    <t>Elective admissions (knee replacement)</t>
+  </si>
+  <si>
+    <t>Elective hospital admissions</t>
+  </si>
+  <si>
+    <t>Elective hospital admissions (coronary heart disease)</t>
+  </si>
+  <si>
+    <t>Elective hospital admissions (hip replacement)</t>
+  </si>
+  <si>
+    <t>Emergency Admissions for injury in children aged 15-24</t>
+  </si>
+  <si>
+    <t>Emergency Admissions for injury in children under 15</t>
+  </si>
+  <si>
+    <t>Emergency Admissions for injury in children under 5</t>
+  </si>
+  <si>
+    <t>Emergency hospital admissions</t>
+  </si>
+  <si>
+    <t>Emergency hospital admissions (coronary heart disease)</t>
+  </si>
+  <si>
+    <t>Emergency hospital admissions, Chronic Obstructive Pulmonary Disease (COPD)</t>
+  </si>
+  <si>
+    <t>Emergency hospital admissions, Myocardial Infarction</t>
+  </si>
+  <si>
+    <t>Emergency hospital admissions, Stroke</t>
+  </si>
+  <si>
+    <t>Emergency hospital admissions, hip fracture in 65+</t>
+  </si>
+  <si>
+    <t>Epilepsy prevalence</t>
+  </si>
+  <si>
+    <t>Fair health</t>
+  </si>
+  <si>
+    <t>Female healthy life expectancy at birth</t>
+  </si>
+  <si>
+    <t>Female life expectancy at birth</t>
+  </si>
+  <si>
+    <t>Fertility rate</t>
+  </si>
+  <si>
+    <t>Good health</t>
+  </si>
+  <si>
+    <t>Grants issued in response to COVID-19</t>
+  </si>
+  <si>
+    <t>Healthy eating</t>
+  </si>
+  <si>
+    <t>Heart Failure prevalence</t>
+  </si>
+  <si>
+    <t>High Blood Pressure prevalence</t>
+  </si>
+  <si>
+    <t>Hospital admissions for alcohol attributable harm</t>
+  </si>
+  <si>
+    <t>Hospital stays for intentional self harm</t>
+  </si>
+  <si>
+    <t>Incidence of breast cancer</t>
+  </si>
+  <si>
+    <t>Incidence of colorectal cancer</t>
+  </si>
+  <si>
+    <t>Incidence of lung cancer</t>
+  </si>
+  <si>
+    <t>Incidence of prostate cancer</t>
+  </si>
+  <si>
+    <t>Learning Disabilities prevalence</t>
+  </si>
+  <si>
+    <t>Live births</t>
+  </si>
+  <si>
+    <t>Low birth weight</t>
+  </si>
+  <si>
+    <t>Male healthy life expectancy at birth</t>
+  </si>
+  <si>
+    <t>Male life expectancy at birth</t>
+  </si>
+  <si>
+    <t>Modelled prevalence of people aged 15 who are regular or occasional smokers</t>
+  </si>
+  <si>
+    <t>Modelled prevalence of people aged 15 who are regular smokers</t>
+  </si>
+  <si>
+    <t>Modelled prevalence of people aged 15 who have never smoked</t>
+  </si>
+  <si>
+    <t>Obese adults</t>
+  </si>
+  <si>
+    <t>Obese children in reception year</t>
+  </si>
+  <si>
+    <t>Obese children in year 6</t>
+  </si>
+  <si>
+    <t>Obesity prevalence</t>
+  </si>
+  <si>
+    <t>One person in household with a long-term health problem or disability: No dependent children</t>
+  </si>
+  <si>
+    <t>One person in household with a long-term health problem or disability: With dependent children</t>
+  </si>
+  <si>
+    <t>Osteoporosis prevalence</t>
+  </si>
+  <si>
+    <t>Overweight or obese children in reception year</t>
+  </si>
+  <si>
+    <t>Overweight or obese children in year 6</t>
+  </si>
+  <si>
+    <t>Palliative Care prevalence</t>
+  </si>
+  <si>
+    <t>People over the age of 65 with bad or very bad health</t>
+  </si>
+  <si>
+    <t>People who participate in sport and physical activity at least twice in the last 28 days (2016/17)</t>
+  </si>
+  <si>
+    <t>People who participate in sport and physical activity at least twice in the last 28 days (2017/18)</t>
+  </si>
+  <si>
+    <t>People who participate in sport and physical activity at least twice in the last 28 days (2018/19)</t>
+  </si>
+  <si>
+    <t>People with a limiting long-term illness (aged 16-64)</t>
+  </si>
+  <si>
+    <t>People with a limiting long-term illness (aged 65+)</t>
+  </si>
+  <si>
+    <t>People with a limiting long-term illness aged 0-15</t>
+  </si>
+  <si>
+    <t>People with a limiting long-term illness aged 16-24</t>
+  </si>
+  <si>
+    <t>Percentage of people aged 45+ with hip osteoarthritis</t>
+  </si>
+  <si>
+    <t>Percentage of people aged 45+ with knee osteoarthritis</t>
+  </si>
+  <si>
+    <t>Percentage of people aged 45+ with severe hip osteoarthritis</t>
+  </si>
+  <si>
+    <t>Percentage of people aged 45+ with severe knee osteoarthritis</t>
+  </si>
+  <si>
+    <t>Percentage of people with back pain</t>
+  </si>
+  <si>
+    <t>Percentage of people with severe back pain</t>
+  </si>
+  <si>
+    <t>Probability of loneliness for those aged 65 and over</t>
+  </si>
+  <si>
+    <t>Proportion of people with high happiness (happiness score of 7-8 where 0 is 'not at all happy' and 10 is 'completely happy')</t>
+  </si>
+  <si>
+    <t>Proportion of people with high life satisfaction (life satisfaction score of 7-8 where 0 is 'not at all satisfied' and 10 is 'completely satisfied')</t>
+  </si>
+  <si>
+    <t>Proportion of people with high sense of self-worth (worthwhile score of 7-8 where 0 is 'not at all worthwhile' and 10 is 'completely worthwhile')</t>
+  </si>
+  <si>
+    <t>Proportion of people with low anxiety (anxiety score of 2-3 where 0 is 'not at all anxious' and 10 is 'completely anxious')</t>
+  </si>
+  <si>
+    <t>Proportion of people with low happiness (happiness score of 0-4 where 0 is 'not at all happy' and 10 is 'completely happy')</t>
+  </si>
+  <si>
+    <t>Proportion of people with low life satisfaction (life satisfaction score of 0-4 where 0 is 'not at all satisfied' and 10 is 'completely satisfied')</t>
+  </si>
+  <si>
+    <t>Proportion of people with low sense of self-worth (worthwhile score of 0-4 where 0 is 'not at all worthwhile' and 10 is 'completely worthwhile')</t>
+  </si>
+  <si>
+    <t>Proportion of people with medium anxiety (anxiety score of 4-5 where 0 is 'not at all anxious' and 10 is 'completely anxious')</t>
+  </si>
+  <si>
+    <t>Proportion of people with medium happiness (happiness score of 5-6 where 0 is 'not at all happy' and 10 is 'completely happy')</t>
+  </si>
+  <si>
+    <t>Proportion of people with medium life satisfaction (life satisfaction score of 5-6 where 0 is 'not at all satisfied' and 10 is 'completely satisfied')</t>
+  </si>
+  <si>
+    <t>Proportion of people with medium sense of self-worth (worthwhile score of 5-6 where 0 is 'not at all worthwhile' and 10 is 'completely worthwhile')</t>
+  </si>
+  <si>
+    <t>Proportion of people with very high happiness (happiness score of 9-10 where 0 is 'not at all happy' and 10 is 'completely happy')</t>
+  </si>
+  <si>
+    <t>Proportion of people with very high life satisfaction (life satisfaction score of 9-10 where 0 is 'not at all satisfied' and 10 is 'completely satisfied')</t>
+  </si>
+  <si>
+    <t>Proportion of people with very high sense of self-worth (worthwhile score of 9-10 where 0 is 'not at all worthwhile' and 10 is 'completely worthwhile')</t>
+  </si>
+  <si>
+    <t>Proportion of people with very low anxiety (anxiety score of 0-1 where 0 is 'not at all anxious' and 10 is 'completely anxious')</t>
+  </si>
+  <si>
+    <t>Rate of A&amp;E attendance for children under 5</t>
+  </si>
+  <si>
+    <t>Rate of emergency hospital admissions for children under 5</t>
+  </si>
+  <si>
+    <t>Rheumatoid Arthritis prevalence</t>
+  </si>
+  <si>
+    <t>Road accident casualty rate</t>
+  </si>
+  <si>
+    <t>Serious Mental Illness prevalence</t>
+  </si>
+  <si>
+    <t>Small Area Mental Health Index</t>
+  </si>
+  <si>
+    <t>Stroke and Transient Ischaemic Attack prevalence</t>
+  </si>
+  <si>
+    <t>Very bad health</t>
+  </si>
+  <si>
+    <t>Very good health</t>
+  </si>
+  <si>
+    <t>Schizophrenia, bipolar disorder and psychoses prevalence</t>
+  </si>
+  <si>
     <t>population</t>
   </si>
   <si>
@@ -575,246 +1196,6 @@
   </si>
   <si>
     <t>Aged 0-25</t>
-  </si>
-  <si>
-    <t>deprivation</t>
-  </si>
-  <si>
-    <t>Children 0-19 in absolute low-income couple families (as % of all in absolute low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in absolute low-income in-work families (as % of all in absolute low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in absolute low-income lone parent families (as % of all in absolute low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in absolute low-income out of work families (as % of all in absolute low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in relative low-income couple families (as % of all in relative low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in relative low-income in-work families (as % of all in relative low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in relative low-income lone parent families (as % of all in relative low income families)</t>
-  </si>
-  <si>
-    <t>Children 0-19 in relative low-income out of work families (as % of all in relative low income families)</t>
-  </si>
-  <si>
-    <t>Children aged 0-15 in absolute low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 0-15 in poverty</t>
-  </si>
-  <si>
-    <t>Children aged 0-15 in relative low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 0-19 in absolute low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 0-19 in poverty</t>
-  </si>
-  <si>
-    <t>Children aged 0-19 in relative low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 0-4 in absolute low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 0-4 in poverty</t>
-  </si>
-  <si>
-    <t>Children aged 0-4 in relative low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 11-15 in absolute low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 11-15 in poverty</t>
-  </si>
-  <si>
-    <t>Children aged 11-15 in relative low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 16-19 in absolute low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 16-19 in poverty</t>
-  </si>
-  <si>
-    <t>Children aged 16-19 in relative low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 5-10 in absolute low-income families</t>
-  </si>
-  <si>
-    <t>Children aged 5-10 in poverty</t>
-  </si>
-  <si>
-    <t>Children aged 5-10 in relative low-income families</t>
-  </si>
-  <si>
-    <t>Food Vulnerability Index Score</t>
-  </si>
-  <si>
-    <t>Hardship Fund Vulnerability Index Score</t>
-  </si>
-  <si>
-    <t>Households in Fuel Poverty</t>
-  </si>
-  <si>
-    <t>Households in poverty</t>
-  </si>
-  <si>
-    <t>Index of Multiple Deprivation (IMD) 2019 Rank</t>
-  </si>
-  <si>
-    <t>Index of Multiple Deprivation 2019 (IMD) Score</t>
-  </si>
-  <si>
-    <t>IoD 2019 Acute morbidity indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Adult Skills Sub-domain Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Adult skills and English language proficiency indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Air quality indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Barriers to Housing and Services Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Benzene (component of air quality indicator)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Children and Young People Sub-domain Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Comparative illness and disability ratio indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Crime Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Education, Skills and Training Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Employment Score (rate)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Entry to higher education indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Geographical Barriers Sub-domain Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Health Deprivation and Disability Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Homelessness indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Household overcrowding indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Houses without central heating indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Housing affordability indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Housing in poor condition indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Income Deprivation Affecting Children Index (IDACI) Score (rate)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Income Deprivation Affecting Older People (IDAOPI) Score (rate)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Income Score (rate)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Indoors Sub-domain Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Living Environment Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Mood and anxiety disorders indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Nitrogen dioxide (component of air quality indicator)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Outdoors Sub-domain Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Owner-occupation affordability (component of housing affordability indicator)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Particulates (component of air quality indicator)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Private rental affordability (component of housing affordability indicator)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Road distance to a GP surgery indicator (km)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Road distance to a post office indicator (km)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Road distance to a primary school indicator (km)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Road distance to general store or supermarket indicator (km)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Road traffic accidents indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Staying on in education post 16 indicator</t>
-  </si>
-  <si>
-    <t>IoD 2019 Sulphur dioxide (component of air quality indicator)</t>
-  </si>
-  <si>
-    <t>IoD 2019 Wider Barriers Sub-domain Rank</t>
-  </si>
-  <si>
-    <t>IoD 2019 Years of potential life lost indicator</t>
-  </si>
-  <si>
-    <t>Mortgage debt per household</t>
-  </si>
-  <si>
-    <t>Net annual household income estimate</t>
-  </si>
-  <si>
-    <t>Net annual household income estimate after housing costs</t>
-  </si>
-  <si>
-    <t>Net annual household income estimate before housing costs</t>
-  </si>
-  <si>
-    <t>Percentage of children in poverty (after housing costs)</t>
-  </si>
-  <si>
-    <t>Personal debt (unsecured loans) per person aged 18+</t>
-  </si>
-  <si>
-    <t>Social benefits as a percentage of total household income</t>
-  </si>
-  <si>
-    <t>Total annual household income estimate</t>
   </si>
   <si>
     <t>Yes</t>
@@ -1204,19 +1585,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C260"/>
+  <dimension ref="A1:C386"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J224" sqref="J224"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="91.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="133.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1230,7 +1610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1238,7 +1618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1246,7 +1626,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1254,7 +1634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1262,7 +1642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1270,7 +1650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1278,7 +1658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1286,7 +1666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1294,7 +1674,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1302,7 +1682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1342,7 +1722,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1350,7 +1730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1358,7 +1738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1366,7 +1746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1374,7 +1754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1762,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1406,7 +1786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1414,7 +1794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +1802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -1430,7 +1810,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1438,7 +1818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1454,7 +1834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1470,23 +1850,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>3</v>
       </c>
       <c r="B32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1502,7 +1888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1510,7 +1896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1904,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1526,7 +1912,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1534,7 +1920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1542,7 +1928,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1550,7 +1936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1558,7 +1944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1960,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1582,7 +1968,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1590,7 +1976,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1598,7 +1984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1606,7 +1992,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +2000,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1622,7 +2008,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1630,7 +2016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1638,7 +2024,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1646,7 +2032,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1654,7 +2040,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1662,7 +2048,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +2056,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +2064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1686,7 +2072,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1694,7 +2080,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1702,7 +2088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1710,7 +2096,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -1718,7 +2104,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +2112,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1734,7 +2120,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1742,7 +2128,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +2136,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1758,7 +2144,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +2152,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1774,7 +2160,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1782,7 +2168,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1790,7 +2176,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1798,7 +2184,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1806,7 +2192,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +2200,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1822,7 +2208,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1830,7 +2216,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>3</v>
       </c>
@@ -1838,7 +2224,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +2232,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -1854,7 +2240,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>3</v>
       </c>
@@ -1862,823 +2248,823 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="C96" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B99" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B102" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B103" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B107" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B108" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B110" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B115" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B121" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B122" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B124" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B125" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B126" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B127" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B128" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B129" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B130" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B131" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B132" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B133" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B134" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B135" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B136" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B137" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B138" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B139" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B141" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B143" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B144" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B145" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B146" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B147" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B148" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B149" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B150" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B151" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B152" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B153" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B154" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B155" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B156" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B157" t="s">
-        <v>159</v>
-      </c>
-      <c r="C157" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B158" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B159" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B160" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B161" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B162" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B163" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B164" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B165" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B166" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B167" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+      <c r="C167" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B168" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B169" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B170" t="s">
-        <v>172</v>
-      </c>
-      <c r="C170" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B171" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B172" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B173" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B174" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B175" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B176" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B177" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B178" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B179" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B180" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B181" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B182" t="s">
         <v>185</v>
@@ -2686,7 +3072,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B183" t="s">
         <v>186</v>
@@ -2694,7 +3080,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B184" t="s">
         <v>187</v>
@@ -2702,7 +3088,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B185" t="s">
         <v>188</v>
@@ -2710,7 +3096,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B186" t="s">
         <v>189</v>
@@ -2718,7 +3104,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B187" t="s">
         <v>190</v>
@@ -2726,7 +3112,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B188" t="s">
         <v>191</v>
@@ -2734,7 +3120,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B189" t="s">
         <v>192</v>
@@ -2742,7 +3128,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B190" t="s">
         <v>193</v>
@@ -2750,7 +3136,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B191" t="s">
         <v>194</v>
@@ -2758,7 +3144,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B192" t="s">
         <v>195</v>
@@ -2766,7 +3152,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B193" t="s">
         <v>196</v>
@@ -2774,7 +3160,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B194" t="s">
         <v>197</v>
@@ -2782,7 +3168,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B195" t="s">
         <v>198</v>
@@ -2790,7 +3176,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B196" t="s">
         <v>199</v>
@@ -2798,7 +3184,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B197" t="s">
         <v>200</v>
@@ -2806,7 +3192,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B198" t="s">
         <v>201</v>
@@ -2814,7 +3200,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B199" t="s">
         <v>202</v>
@@ -2822,7 +3208,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B200" t="s">
         <v>203</v>
@@ -2830,7 +3216,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B201" t="s">
         <v>204</v>
@@ -2838,7 +3224,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B202" t="s">
         <v>205</v>
@@ -2846,7 +3232,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B203" t="s">
         <v>206</v>
@@ -2854,7 +3240,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B204" t="s">
         <v>207</v>
@@ -2862,7 +3248,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B205" t="s">
         <v>208</v>
@@ -2870,7 +3256,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B206" t="s">
         <v>209</v>
@@ -2878,447 +3264,1452 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B207" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B208" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B209" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B210" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B213" t="s">
-        <v>216</v>
-      </c>
-      <c r="C213" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B214" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B215" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B216" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B217" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B218" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B219" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B220" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B221" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B222" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B223" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B224" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B225" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B226" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B227" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B228" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B229" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B230" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B231" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B232" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B233" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B234" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B235" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B236" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B237" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B238" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B239" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B240" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B241" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B242" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B243" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B244" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B245" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B246" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B247" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B248" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B249" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B250" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B251" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B252" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B253" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B254" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B255" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B256" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B257" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B258" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B259" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="B260" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>210</v>
+      </c>
+      <c r="B261" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>210</v>
+      </c>
+      <c r="B262" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>210</v>
+      </c>
+      <c r="B263" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>210</v>
+      </c>
+      <c r="B264" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>210</v>
+      </c>
+      <c r="B265" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>210</v>
+      </c>
+      <c r="B266" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>210</v>
+      </c>
+      <c r="B267" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>210</v>
+      </c>
+      <c r="B268" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>210</v>
+      </c>
+      <c r="B269" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>210</v>
+      </c>
+      <c r="B270" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>210</v>
+      </c>
+      <c r="B271" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>210</v>
+      </c>
+      <c r="B272" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>210</v>
+      </c>
+      <c r="B273" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>210</v>
+      </c>
+      <c r="B274" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>210</v>
+      </c>
+      <c r="B275" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>210</v>
+      </c>
+      <c r="B276" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>210</v>
+      </c>
+      <c r="B277" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>210</v>
+      </c>
+      <c r="B278" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>210</v>
+      </c>
+      <c r="B279" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>210</v>
+      </c>
+      <c r="B280" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>210</v>
+      </c>
+      <c r="B281" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>210</v>
+      </c>
+      <c r="B282" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>210</v>
+      </c>
+      <c r="B283" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>210</v>
+      </c>
+      <c r="B284" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>210</v>
+      </c>
+      <c r="B285" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>210</v>
+      </c>
+      <c r="B286" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>210</v>
+      </c>
+      <c r="B287" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>210</v>
+      </c>
+      <c r="B288" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>210</v>
+      </c>
+      <c r="B289" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>210</v>
+      </c>
+      <c r="B290" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>210</v>
+      </c>
+      <c r="B291" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>210</v>
+      </c>
+      <c r="B292" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>210</v>
+      </c>
+      <c r="B293" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>210</v>
+      </c>
+      <c r="B294" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>210</v>
+      </c>
+      <c r="B295" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>210</v>
+      </c>
+      <c r="B296" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>210</v>
+      </c>
+      <c r="B297" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>210</v>
+      </c>
+      <c r="B298" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>210</v>
+      </c>
+      <c r="B299" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>210</v>
+      </c>
+      <c r="B300" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>210</v>
+      </c>
+      <c r="B301" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>210</v>
+      </c>
+      <c r="B302" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>210</v>
+      </c>
+      <c r="B303" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>210</v>
+      </c>
+      <c r="B304" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>210</v>
+      </c>
+      <c r="B305" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>210</v>
+      </c>
+      <c r="B306" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>210</v>
+      </c>
+      <c r="B307" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>210</v>
+      </c>
+      <c r="B308" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>210</v>
+      </c>
+      <c r="B309" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>210</v>
+      </c>
+      <c r="B310" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>210</v>
+      </c>
+      <c r="B311" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>210</v>
+      </c>
+      <c r="B312" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>210</v>
+      </c>
+      <c r="B313" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>210</v>
+      </c>
+      <c r="B314" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>210</v>
+      </c>
+      <c r="B315" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>210</v>
+      </c>
+      <c r="B316" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>210</v>
+      </c>
+      <c r="B317" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>210</v>
+      </c>
+      <c r="B318" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>210</v>
+      </c>
+      <c r="B319" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>210</v>
+      </c>
+      <c r="B320" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>210</v>
+      </c>
+      <c r="B321" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>210</v>
+      </c>
+      <c r="B322" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>210</v>
+      </c>
+      <c r="B323" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>210</v>
+      </c>
+      <c r="B324" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>210</v>
+      </c>
+      <c r="B325" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>210</v>
+      </c>
+      <c r="B326" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>210</v>
+      </c>
+      <c r="B327" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>210</v>
+      </c>
+      <c r="B328" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>210</v>
+      </c>
+      <c r="B329" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>210</v>
+      </c>
+      <c r="B330" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>210</v>
+      </c>
+      <c r="B331" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>210</v>
+      </c>
+      <c r="B332" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>210</v>
+      </c>
+      <c r="B333" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>210</v>
+      </c>
+      <c r="B334" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>210</v>
+      </c>
+      <c r="B335" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>210</v>
+      </c>
+      <c r="B336" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>210</v>
+      </c>
+      <c r="B337" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>210</v>
+      </c>
+      <c r="B338" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>210</v>
+      </c>
+      <c r="B339" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>210</v>
+      </c>
+      <c r="B340" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>210</v>
+      </c>
+      <c r="B341" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>210</v>
+      </c>
+      <c r="B342" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>210</v>
+      </c>
+      <c r="B343" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>210</v>
+      </c>
+      <c r="B344" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>210</v>
+      </c>
+      <c r="B345" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>210</v>
+      </c>
+      <c r="B346" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>210</v>
+      </c>
+      <c r="B347" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>210</v>
+      </c>
+      <c r="B348" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>210</v>
+      </c>
+      <c r="B349" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>210</v>
+      </c>
+      <c r="B350" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>210</v>
+      </c>
+      <c r="B351" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>210</v>
+      </c>
+      <c r="B352" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>210</v>
+      </c>
+      <c r="B353" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>210</v>
+      </c>
+      <c r="B354" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>210</v>
+      </c>
+      <c r="B355" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>210</v>
+      </c>
+      <c r="B356" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>210</v>
+      </c>
+      <c r="B357" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>210</v>
+      </c>
+      <c r="B358" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>210</v>
+      </c>
+      <c r="B359" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>210</v>
+      </c>
+      <c r="B360" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>210</v>
+      </c>
+      <c r="B361" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>210</v>
+      </c>
+      <c r="B362" t="s">
+        <v>366</v>
+      </c>
+      <c r="C362" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>210</v>
+      </c>
+      <c r="B363" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>210</v>
+      </c>
+      <c r="B364" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>210</v>
+      </c>
+      <c r="B365" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>210</v>
+      </c>
+      <c r="B366" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>210</v>
+      </c>
+      <c r="B367" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>210</v>
+      </c>
+      <c r="B368" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>210</v>
+      </c>
+      <c r="B369" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>210</v>
+      </c>
+      <c r="B370" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>210</v>
+      </c>
+      <c r="B371" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>210</v>
+      </c>
+      <c r="B372" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>210</v>
+      </c>
+      <c r="B373" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>210</v>
+      </c>
+      <c r="B374" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>210</v>
+      </c>
+      <c r="B375" t="s">
+        <v>379</v>
+      </c>
+      <c r="C375" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>210</v>
+      </c>
+      <c r="B376" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>210</v>
+      </c>
+      <c r="B377" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>210</v>
+      </c>
+      <c r="B378" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>210</v>
+      </c>
+      <c r="B379" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>210</v>
+      </c>
+      <c r="B380" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>210</v>
+      </c>
+      <c r="B381" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>210</v>
+      </c>
+      <c r="B382" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="383" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>210</v>
+      </c>
+      <c r="B383" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="384" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>210</v>
+      </c>
+      <c r="B384" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>210</v>
+      </c>
+      <c r="B385" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>210</v>
+      </c>
+      <c r="B386" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C260" xr:uid="{EF5AA1A9-BF36-4E01-8C1C-DF384EC058C4}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="deprivation"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C386" xr:uid="{ED44AD21-424B-4A23-97A1-8AC2C0B1EF3E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The "Serious Mental Illness prevalence" indicator needs to be identified as type "small percentage" so that it can be formatted correctly.
</commit_message>
<xml_diff>
--- a/sli_measures.xlsx
+++ b/sli_measures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa0eda03202f8011/BI/Repo/asc-localities-insight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_5E597DCC8F79A8D366075C52F37BD272AA4CE64B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9C1A0DE-EE1C-439E-83F9-F7102A1DD989}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_5E597DCC8F79A8D366075C52F37BD272AA4CE64B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88912322-F84B-49D6-8720-E610BD2A6800}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="-108" windowWidth="22704" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57120" yWindow="-120" windowWidth="28440" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3105,7 +3105,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D886" sqref="D886"/>
+      <selection pane="bottomLeft" activeCell="B889" sqref="B889"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8285,7 +8285,7 @@
         <v>892</v>
       </c>
       <c r="D639" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
     </row>
     <row r="640" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixes #17. Significant rewrite.
</commit_message>
<xml_diff>
--- a/sli_measures.xlsx
+++ b/sli_measures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa0eda03202f8011/BI/Repo/asc-localities-insight/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_5E597DCC8F79A8D366075C52F37BD272AA4CE64B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88912322-F84B-49D6-8720-E610BD2A6800}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="11_5E597DCC8F79A8D366075C52F37BD272AA4CE64B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E8FF181-3F4A-4783-9099-8B92E90FD042}"/>
   <bookViews>
     <workbookView xWindow="-57120" yWindow="-120" windowWidth="28440" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$881</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$881</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="897">
   <si>
     <t>theme</t>
   </si>
@@ -2710,10 +2710,10 @@
     <t>percentage</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>small percentage</t>
+    <t>decimals</t>
+  </si>
+  <si>
+    <t>numeric</t>
   </si>
 </sst>
 </file>
@@ -3101,11 +3101,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D881"/>
+  <dimension ref="A1:E881"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B889" sqref="B889"/>
+      <selection pane="bottomLeft" activeCell="E890" sqref="E890"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3114,9 +3114,10 @@
     <col min="2" max="2" width="133.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3129,8 +3130,11 @@
       <c r="D1" s="1" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3138,7 +3142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3146,7 +3150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3162,7 +3166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3170,7 +3174,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -3178,7 +3182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -3186,7 +3190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -3194,7 +3198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3202,7 +3206,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -3210,7 +3214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3218,7 +3222,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3226,7 +3230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3234,7 +3238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -3242,7 +3246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -3378,7 +3382,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -3386,7 +3390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -3394,7 +3398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -3402,7 +3406,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -3410,7 +3414,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -3418,7 +3422,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -3426,7 +3430,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -3434,7 +3438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -3447,8 +3451,11 @@
       <c r="D40" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -3456,7 +3463,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -3464,7 +3471,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -3472,7 +3479,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -3480,7 +3487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -3488,7 +3495,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -3496,7 +3503,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -3504,7 +3511,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -3768,7 +3775,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -3776,7 +3783,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -3784,7 +3791,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -3792,7 +3799,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>3</v>
       </c>
@@ -3800,7 +3807,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>3</v>
       </c>
@@ -3808,7 +3815,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>3</v>
       </c>
@@ -3816,7 +3823,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -3824,7 +3831,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -3832,7 +3839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -3840,7 +3847,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -3853,8 +3860,11 @@
       <c r="D90" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>3</v>
       </c>
@@ -3862,7 +3872,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>3</v>
       </c>
@@ -3870,7 +3880,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -3878,7 +3888,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -3891,8 +3901,11 @@
       <c r="D94" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -3900,7 +3913,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -4420,7 +4433,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>148</v>
       </c>
@@ -4428,7 +4441,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>148</v>
       </c>
@@ -4436,7 +4449,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>148</v>
       </c>
@@ -4444,7 +4457,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>148</v>
       </c>
@@ -4452,7 +4465,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>148</v>
       </c>
@@ -4460,7 +4473,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>148</v>
       </c>
@@ -4468,7 +4481,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>148</v>
       </c>
@@ -4476,7 +4489,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>148</v>
       </c>
@@ -4484,7 +4497,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>148</v>
       </c>
@@ -4492,7 +4505,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>148</v>
       </c>
@@ -4500,7 +4513,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>148</v>
       </c>
@@ -4508,7 +4521,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>148</v>
       </c>
@@ -4516,7 +4529,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>148</v>
       </c>
@@ -4524,7 +4537,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>148</v>
       </c>
@@ -4532,7 +4545,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>148</v>
       </c>
@@ -4543,10 +4556,13 @@
         <v>892</v>
       </c>
       <c r="D175" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+        <v>896</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>148</v>
       </c>
@@ -4557,7 +4573,10 @@
         <v>892</v>
       </c>
       <c r="D176" t="s">
-        <v>895</v>
+        <v>896</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -7376,7 +7395,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="529" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>526</v>
       </c>
@@ -7384,7 +7403,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="530" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A530" t="s">
         <v>526</v>
       </c>
@@ -7392,7 +7411,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="531" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>526</v>
       </c>
@@ -7400,7 +7419,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="532" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A532" t="s">
         <v>526</v>
       </c>
@@ -7408,7 +7427,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="533" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>526</v>
       </c>
@@ -7416,7 +7435,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="534" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A534" t="s">
         <v>526</v>
       </c>
@@ -7427,10 +7446,13 @@
         <v>892</v>
       </c>
       <c r="D534" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="535" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>896</v>
+      </c>
+      <c r="E534">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>526</v>
       </c>
@@ -7438,7 +7460,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="536" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A536" t="s">
         <v>526</v>
       </c>
@@ -7446,7 +7468,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="537" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>526</v>
       </c>
@@ -7454,7 +7476,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="538" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A538" t="s">
         <v>526</v>
       </c>
@@ -7462,7 +7484,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="539" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>526</v>
       </c>
@@ -7470,7 +7492,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="540" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A540" t="s">
         <v>526</v>
       </c>
@@ -7478,7 +7500,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="541" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>526</v>
       </c>
@@ -7486,7 +7508,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="542" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A542" t="s">
         <v>526</v>
       </c>
@@ -7494,7 +7516,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="543" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>526</v>
       </c>
@@ -7502,7 +7524,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="544" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A544" t="s">
         <v>526</v>
       </c>
@@ -7766,7 +7788,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="577" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>526</v>
       </c>
@@ -7774,7 +7796,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="578" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A578" t="s">
         <v>526</v>
       </c>
@@ -7782,7 +7804,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="579" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>526</v>
       </c>
@@ -7790,7 +7812,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="580" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A580" t="s">
         <v>526</v>
       </c>
@@ -7798,7 +7820,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="581" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>526</v>
       </c>
@@ -7806,7 +7828,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="582" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A582" t="s">
         <v>526</v>
       </c>
@@ -7814,7 +7836,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="583" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>526</v>
       </c>
@@ -7822,7 +7844,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="584" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>526</v>
       </c>
@@ -7830,7 +7852,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="585" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>526</v>
       </c>
@@ -7838,7 +7860,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="586" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A586" t="s">
         <v>526</v>
       </c>
@@ -7846,7 +7868,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="587" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>526</v>
       </c>
@@ -7857,10 +7879,13 @@
         <v>892</v>
       </c>
       <c r="D587" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="588" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>894</v>
+      </c>
+      <c r="E587">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A588" t="s">
         <v>526</v>
       </c>
@@ -7868,7 +7893,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="589" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>526</v>
       </c>
@@ -7876,7 +7901,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="590" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A590" t="s">
         <v>526</v>
       </c>
@@ -7884,7 +7909,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="591" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>526</v>
       </c>
@@ -7892,7 +7917,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="592" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A592" t="s">
         <v>526</v>
       </c>
@@ -7900,7 +7925,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="593" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>526</v>
       </c>
@@ -7908,7 +7933,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="594" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A594" t="s">
         <v>526</v>
       </c>
@@ -7916,7 +7941,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="595" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>526</v>
       </c>
@@ -7924,7 +7949,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="596" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A596" t="s">
         <v>526</v>
       </c>
@@ -7932,7 +7957,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="597" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>526</v>
       </c>
@@ -7940,7 +7965,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="598" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A598" t="s">
         <v>526</v>
       </c>
@@ -7948,7 +7973,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="599" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>526</v>
       </c>
@@ -7956,7 +7981,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="600" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A600" t="s">
         <v>526</v>
       </c>
@@ -7964,7 +7989,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="601" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>526</v>
       </c>
@@ -7972,7 +7997,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="602" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
         <v>526</v>
       </c>
@@ -7980,7 +8005,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="603" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>526</v>
       </c>
@@ -7988,7 +8013,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="604" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A604" t="s">
         <v>526</v>
       </c>
@@ -7996,7 +8021,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="605" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>526</v>
       </c>
@@ -8009,8 +8034,11 @@
       <c r="D605" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="606" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E605">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A606" t="s">
         <v>526</v>
       </c>
@@ -8018,7 +8046,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="607" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>526</v>
       </c>
@@ -8026,7 +8054,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="608" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A608" t="s">
         <v>526</v>
       </c>
@@ -8162,7 +8190,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="625" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
         <v>526</v>
       </c>
@@ -8170,7 +8198,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="626" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="626" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A626" t="s">
         <v>526</v>
       </c>
@@ -8178,7 +8206,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="627" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="627" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
         <v>526</v>
       </c>
@@ -8186,7 +8214,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="628" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="628" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A628" t="s">
         <v>526</v>
       </c>
@@ -8194,7 +8222,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="629" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="629" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
         <v>526</v>
       </c>
@@ -8202,7 +8230,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="630" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="630" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A630" t="s">
         <v>526</v>
       </c>
@@ -8210,7 +8238,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="631" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="631" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
         <v>526</v>
       </c>
@@ -8218,7 +8246,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="632" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A632" t="s">
         <v>526</v>
       </c>
@@ -8226,7 +8254,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="633" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
         <v>526</v>
       </c>
@@ -8234,7 +8262,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="634" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="634" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A634" t="s">
         <v>526</v>
       </c>
@@ -8242,7 +8270,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="635" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
         <v>526</v>
       </c>
@@ -8250,7 +8278,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="636" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A636" t="s">
         <v>526</v>
       </c>
@@ -8258,7 +8286,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="637" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="637" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
         <v>526</v>
       </c>
@@ -8266,7 +8294,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="638" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="638" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A638" t="s">
         <v>526</v>
       </c>
@@ -8274,7 +8302,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="639" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="639" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
         <v>526</v>
       </c>
@@ -8285,10 +8313,13 @@
         <v>892</v>
       </c>
       <c r="D639" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="640" spans="1:4" x14ac:dyDescent="0.3">
+        <v>894</v>
+      </c>
+      <c r="E639">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="640" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A640" t="s">
         <v>526</v>
       </c>
@@ -8299,7 +8330,10 @@
         <v>892</v>
       </c>
       <c r="D640" t="s">
-        <v>895</v>
+        <v>896</v>
+      </c>
+      <c r="E640">
+        <v>0</v>
       </c>
     </row>
     <row r="641" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
@@ -9454,7 +9488,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="785" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="785" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
         <v>653</v>
       </c>
@@ -9462,7 +9496,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="786" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="786" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A786" t="s">
         <v>653</v>
       </c>
@@ -9470,7 +9504,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="787" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="787" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A787" t="s">
         <v>653</v>
       </c>
@@ -9478,7 +9512,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="788" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="788" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A788" t="s">
         <v>653</v>
       </c>
@@ -9486,7 +9520,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="789" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="789" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A789" t="s">
         <v>653</v>
       </c>
@@ -9494,7 +9528,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="790" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="790" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A790" t="s">
         <v>653</v>
       </c>
@@ -9502,7 +9536,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="791" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="791" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A791" t="s">
         <v>653</v>
       </c>
@@ -9510,7 +9544,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="792" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="792" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A792" t="s">
         <v>653</v>
       </c>
@@ -9518,7 +9552,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="793" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="793" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
         <v>653</v>
       </c>
@@ -9526,7 +9560,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="794" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="794" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
         <v>653</v>
       </c>
@@ -9534,7 +9568,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="795" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="795" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
         <v>653</v>
       </c>
@@ -9542,7 +9576,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="796" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="796" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A796" t="s">
         <v>653</v>
       </c>
@@ -9550,7 +9584,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="797" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="797" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A797" t="s">
         <v>653</v>
       </c>
@@ -9558,7 +9592,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="798" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="798" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A798" t="s">
         <v>653</v>
       </c>
@@ -9566,7 +9600,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="799" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="799" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A799" t="s">
         <v>653</v>
       </c>
@@ -9574,7 +9608,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="800" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="800" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A800" t="s">
         <v>653</v>
       </c>
@@ -9587,8 +9621,11 @@
       <c r="D800" t="s">
         <v>894</v>
       </c>
-    </row>
-    <row r="801" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E800">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="801" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A801" t="s">
         <v>653</v>
       </c>
@@ -9596,7 +9633,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="802" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="802" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A802" t="s">
         <v>653</v>
       </c>
@@ -9604,7 +9641,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="803" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="803" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A803" t="s">
         <v>653</v>
       </c>
@@ -9612,7 +9649,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="804" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="804" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
         <v>653</v>
       </c>
@@ -9620,7 +9657,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="805" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="805" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
         <v>653</v>
       </c>
@@ -9628,7 +9665,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="806" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="806" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A806" t="s">
         <v>653</v>
       </c>
@@ -9636,7 +9673,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="807" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="807" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
         <v>653</v>
       </c>
@@ -9644,7 +9681,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="808" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="808" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
         <v>653</v>
       </c>
@@ -9652,7 +9689,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="809" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="809" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
         <v>653</v>
       </c>
@@ -9660,7 +9697,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="810" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="810" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
         <v>653</v>
       </c>
@@ -9668,7 +9705,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="811" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="811" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
         <v>653</v>
       </c>
@@ -9676,7 +9713,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="812" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="812" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
         <v>653</v>
       </c>
@@ -9684,7 +9721,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="813" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="813" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
         <v>653</v>
       </c>
@@ -9695,10 +9732,13 @@
         <v>892</v>
       </c>
       <c r="D813" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="814" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>896</v>
+      </c>
+      <c r="E813">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
         <v>653</v>
       </c>
@@ -9706,7 +9746,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="815" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="815" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
         <v>653</v>
       </c>
@@ -9714,7 +9754,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="816" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="816" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
         <v>653</v>
       </c>
@@ -10243,7 +10283,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D881" xr:uid="{BF2CDFDA-3CC0-4E62-B210-27CF275B3072}">
+  <autoFilter ref="A1:E881" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="2">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>

</xml_diff>